<commit_message>
Dataset Log-trasformato Scalato XGBoost scelto
</commit_message>
<xml_diff>
--- a/risultati_alle_mod_K.xlsx
+++ b/risultati_alle_mod_K.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,28 +487,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08694692721978813</v>
+        <v>0.09482646153591366</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007559768152963134</v>
+        <v>0.008992057807422113</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8051089035470875</v>
+        <v>0.7336261084701818</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02494723840470688</v>
+        <v>0.02312480534815172</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0006223647040212818</v>
+        <v>0.0005347566223899063</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9597137886283112</v>
+        <v>0.9847742714255313</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001000642776489258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -518,28 +518,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C3" t="n">
-        <v>0.11522571036204</v>
+        <v>0.1195654240444575</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01327696432843673</v>
+        <v>0.01429589062693093</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6067196003560357</v>
+        <v>0.6314514225018637</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05682387964657178</v>
+        <v>0.03873184960659918</v>
       </c>
       <c r="G3" t="n">
-        <v>0.003228953298088074</v>
+        <v>0.001500156173948217</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9080419843122589</v>
+        <v>0.9028935794091193</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.002990961074829102</v>
       </c>
     </row>
     <row r="4">
@@ -552,25 +552,25 @@
         <v>57</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1837376861685028</v>
+        <v>0.18373768617052</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03375953731855524</v>
+        <v>0.03375953731929648</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1873855451427607</v>
+        <v>0.1873855451473129</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03511334252844962</v>
+        <v>0.03511334253015564</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.546049066547539e-09</v>
+        <v>-1.546049510636749e-09</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0009999275207519531</v>
+        <v>0.002991437911987305</v>
       </c>
     </row>
     <row r="5">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -592,16 +592,16 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.008803026354384139</v>
+        <v>0.006432844888492792</v>
       </c>
       <c r="G5" t="n">
-        <v>7.749327299598171e-05</v>
+        <v>4.138149335940784e-05</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9949144812564377</v>
+        <v>0.9973213397587389</v>
       </c>
       <c r="I5" t="n">
-        <v>0.00099945068359375</v>
+        <v>0.002347230911254883</v>
       </c>
     </row>
     <row r="6">
@@ -611,28 +611,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0403051708623513</v>
+        <v>0.04631584119436853</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001624506798243332</v>
+        <v>0.002145157145541965</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9600995785302965</v>
+        <v>0.9472750420931946</v>
       </c>
       <c r="F6" t="n">
-        <v>0.004104530930429968</v>
+        <v>0.002916006050421347</v>
       </c>
       <c r="G6" t="n">
-        <v>1.68471741588563e-05</v>
+        <v>8.503091286093906e-06</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9976975955842881</v>
+        <v>0.998845769281683</v>
       </c>
       <c r="I6" t="n">
-        <v>0.05651211738586426</v>
+        <v>0.1521124839782715</v>
       </c>
     </row>
     <row r="7">
@@ -642,28 +642,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C7" t="n">
-        <v>0.11243933400719</v>
+        <v>0.1372283170240384</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01264260383198043</v>
+        <v>0.01883161099324999</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6119186382835824</v>
+        <v>0.3529241615997377</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07601866315954367</v>
+        <v>0.1036722936857353</v>
       </c>
       <c r="G7" t="n">
-        <v>0.005778837148564161</v>
+        <v>0.01074794447806135</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8477681331021435</v>
+        <v>0.7619592110376481</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.0009980201721191406</v>
       </c>
     </row>
     <row r="8">
@@ -673,28 +673,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C8" t="n">
-        <v>9.633995494185726e-08</v>
+        <v>1.250252383024717e-07</v>
       </c>
       <c r="D8" t="n">
-        <v>9.281386918199088e-15</v>
+        <v>1.563131021258985e-14</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9999999999997607</v>
+        <v>0.9999999999995979</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0202581527610477</v>
+        <v>0.03445772132397083</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0004103927532899443</v>
+        <v>0.001187334558840434</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9734349183081523</v>
+        <v>0.922292498210229</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0009996891021728516</v>
+        <v>0.00197148323059082</v>
       </c>
     </row>
     <row r="9">
@@ -704,28 +704,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09131469802400242</v>
+        <v>0.1061764900883697</v>
       </c>
       <c r="D9" t="n">
-        <v>0.008338374075214752</v>
+        <v>0.01127344704748566</v>
       </c>
       <c r="E9" t="n">
-        <v>0.753006861541561</v>
+        <v>0.6864283876845669</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02335950910691198</v>
+        <v>0.03742826243096131</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0005456666657159038</v>
+        <v>0.00140087482860091</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9844598483861963</v>
+        <v>0.9468672020306033</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00500035285949707</v>
+        <v>0.01784348487854004</v>
       </c>
     </row>
     <row r="10">
@@ -735,28 +735,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0008665248161570093</v>
+        <v>0.0007202721970399165</v>
       </c>
       <c r="D10" t="n">
-        <v>7.508652570159388e-07</v>
+        <v>5.187920378287083e-07</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9999808663892907</v>
+        <v>0.9999866255224982</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02000828433328842</v>
+        <v>0.006526189894802719</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0004003314419617148</v>
+        <v>4.259115454302513e-05</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9713448644927261</v>
+        <v>0.9972430373328257</v>
       </c>
       <c r="I10" t="n">
-        <v>0.03000020980834961</v>
+        <v>0.04020166397094727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>